<commit_message>
Added constraints and elems of risks + team members names
</commit_message>
<xml_diff>
--- a/doc/work_log.xlsx
+++ b/doc/work_log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-120" windowWidth="25600" windowHeight="15100" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Who?</t>
   </si>
@@ -755,7 +755,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -961,11 +961,21 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="A12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="10">
+        <v>42450</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6"/>

</xml_diff>

<commit_message>
Learning video processing with Matlab
</commit_message>
<xml_diff>
--- a/doc/work_log.xlsx
+++ b/doc/work_log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>Who?</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Worked on slides</t>
+  </si>
+  <si>
+    <t>Learning to use Matlab for video processing</t>
   </si>
 </sst>
 </file>
@@ -755,7 +758,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -978,11 +981,21 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="A13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="10">
+        <v>42450</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2"/>

</xml_diff>